<commit_message>
Adding solution for second question.
</commit_message>
<xml_diff>
--- a/01 - SELF-TEST DIAGNOSTIC/Program 01 - 83x8x8/SELF-TEST DIAGNOSTIC.xlsx
+++ b/01 - SELF-TEST DIAGNOSTIC/Program 01 - 83x8x8/SELF-TEST DIAGNOSTIC.xlsx
@@ -20,7 +20,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve">IN X </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">↓</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve">IN A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">↓</t>
+    </r>
+  </si>
   <si>
     <t xml:space="preserve">MOV UP, DOWN</t>
   </si>
@@ -36,6 +78,50 @@
   <si>
     <t xml:space="preserve">MOV LEFT, DOWN</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve">OUT X </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">↓</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve">OUT A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">↓</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -44,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -68,6 +154,26 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,9 +239,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -159,6 +269,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -173,9 +343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>15840</xdr:colOff>
+      <xdr:colOff>15120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -188,8 +358,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2915280" y="487800"/>
-          <a:ext cx="2134800" cy="2275560"/>
+          <a:off x="3071520" y="487800"/>
+          <a:ext cx="2347200" cy="2274840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -210,9 +380,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>25200</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -225,8 +395,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2924640" y="3413880"/>
-          <a:ext cx="2134800" cy="2275560"/>
+          <a:off x="3138120" y="3413880"/>
+          <a:ext cx="2289960" cy="2274840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -247,9 +417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>25200</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -262,8 +432,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2924640" y="6339960"/>
-          <a:ext cx="2134800" cy="2275560"/>
+          <a:off x="3138120" y="6339960"/>
+          <a:ext cx="2289960" cy="2274840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -284,9 +454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>27720</xdr:colOff>
+      <xdr:colOff>27000</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -299,8 +469,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8774280" y="3413880"/>
-          <a:ext cx="2134800" cy="2275560"/>
+          <a:off x="9414360" y="3413880"/>
+          <a:ext cx="2289960" cy="2274840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -320,293 +490,319 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:G53"/>
+  <dimension ref="A2:G54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.9132653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.9132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3316326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.3316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.3316326530612"/>
   </cols>
   <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="A23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="A24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="A25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="A26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="A27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="A29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="A30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="A31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="A32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="A33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="A34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="A35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="E40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>4</v>
+      <c r="A40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="A41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="A42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="A43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="A44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="A46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="A47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="A48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="A49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="A50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="A51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="A52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="A53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="G53" s="4"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="G54:G55"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding 3rd and 4th solutions
</commit_message>
<xml_diff>
--- a/01 - SELF-TEST DIAGNOSTIC/Program 01 - 83x8x8/SELF-TEST DIAGNOSTIC.xlsx
+++ b/01 - SELF-TEST DIAGNOSTIC/Program 01 - 83x8x8/SELF-TEST DIAGNOSTIC.xlsx
@@ -38,6 +38,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">↓</t>
     </r>
@@ -59,6 +60,7 @@
         <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">↓</t>
     </r>
@@ -130,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -161,12 +163,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FFFF3333"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="15"/>
@@ -336,16 +332,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>804600</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1440</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>23760</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -358,45 +354,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3071520" y="487800"/>
-          <a:ext cx="2347200" cy="2274840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>24480</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3138120" y="3413880"/>
-          <a:ext cx="2289960" cy="2274840"/>
+          <a:off x="3360240" y="3413880"/>
+          <a:ext cx="2448360" cy="2274120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -417,23 +376,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>24480</xdr:colOff>
+      <xdr:colOff>23760</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr=""/>
+        <xdr:cNvPr id="1" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3138120" y="6339960"/>
-          <a:ext cx="2289960" cy="2274840"/>
+          <a:off x="3360240" y="6339960"/>
+          <a:ext cx="2448360" cy="2274120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -454,9 +413,46 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>26280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10081080" y="3413880"/>
+          <a:ext cx="2448000" cy="2274120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>22320</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -469,8 +465,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9414360" y="3413880"/>
-          <a:ext cx="2289960" cy="2274840"/>
+          <a:off x="3358800" y="488160"/>
+          <a:ext cx="2448360" cy="2274120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -493,19 +489,19 @@
   <dimension ref="A2:G54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>